<commit_message>
backend for metro rank service
</commit_message>
<xml_diff>
--- a/docs/acronyms.xlsx
+++ b/docs/acronyms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christopher.g\eclipse-workspace\federal_transit\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59BDC38-375D-443B-B2DE-4D5D05DB96D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8F3AEF-CD50-4F2A-A4C4-59BA95B1087D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="2830" windowWidth="16630" windowHeight="5410" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modes" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>LR</t>
   </si>
@@ -110,6 +110,39 @@
   </si>
   <si>
     <t>Taxi</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>Heavy Rail</t>
+  </si>
+  <si>
+    <t>YR</t>
+  </si>
+  <si>
+    <t>Hybrid Rail</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Cable Car</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>Inclined Plane</t>
+  </si>
+  <si>
+    <t>Rail</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Alaska Railroad</t>
   </si>
 </sst>
 </file>
@@ -427,99 +460,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="27.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B16" t="s">
         <v>21</v>
       </c>
     </row>
@@ -532,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA44DA13-F32E-4717-910C-179F5592A34D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
pie chart and stacked bar chart for Metro view
</commit_message>
<xml_diff>
--- a/docs/acronyms.xlsx
+++ b/docs/acronyms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christopher.g\eclipse-workspace\federal_transit\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8F3AEF-CD50-4F2A-A4C4-59BA95B1087D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09506813-03A3-48AC-B34F-2DCA179E3547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>LR</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>Alaska Railroad</t>
+  </si>
+  <si>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>Demand</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,6 +550,9 @@
       <c r="B7" t="s">
         <v>3</v>
       </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -552,6 +561,9 @@
       <c r="B8" t="s">
         <v>5</v>
       </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -560,6 +572,9 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -590,6 +605,9 @@
       <c r="B12" t="s">
         <v>13</v>
       </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -598,6 +616,9 @@
       <c r="B13" t="s">
         <v>15</v>
       </c>
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -614,6 +635,9 @@
       <c r="B15" t="s">
         <v>19</v>
       </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -621,6 +645,9 @@
       </c>
       <c r="B16" t="s">
         <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>